<commit_message>
changed some settings in the input xlsx to make the model feasable! it is still infeasable with EV
</commit_message>
<xml_diff>
--- a/data/input/Scenario_Component_Behavior.xlsx
+++ b/data/input/Scenario_Component_Behavior.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20386"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yus\Documents\code\3E\Flex\data\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mascherbauer\PycharmProjects\NewTrends\Prosumager\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D82B31-974D-4002-A78C-DC23B6D27C47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="24900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OperationScenario_Behavior" sheetId="1" r:id="rId1"/>
@@ -75,8 +76,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -112,7 +113,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -128,24 +129,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:O2" totalsRowShown="0">
-  <autoFilter ref="A1:O2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:O2" totalsRowShown="0">
+  <autoFilter ref="A1:O2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="15">
-    <tableColumn id="1" name="ID_Behavior"/>
-    <tableColumn id="2" name="id_people_at_home_profile"/>
-    <tableColumn id="3" name="target_temperature_at_home_max"/>
-    <tableColumn id="4" name="target_temperature_at_home_min"/>
-    <tableColumn id="5" name="target_temperature_not_at_home_max"/>
-    <tableColumn id="6" name="target_temperature_not_at_home_min"/>
-    <tableColumn id="7" name="temperature_unit"/>
-    <tableColumn id="8" name="id_hot_water_demand_profile"/>
-    <tableColumn id="9" name="hot_water_demand_annual"/>
-    <tableColumn id="10" name="hot_water_demand_unit"/>
-    <tableColumn id="11" name="id_appliance_electricity_demand_profile"/>
-    <tableColumn id="12" name="appliance_electricity_demand_annual"/>
-    <tableColumn id="13" name="appliance_electricity_demand_unit"/>
-    <tableColumn id="14" name="id_vehicle_at_home_profile"/>
-    <tableColumn id="15" name="id_vehicle_distance_profile"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID_Behavior"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="id_people_at_home_profile"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="target_temperature_at_home_max"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="target_temperature_at_home_min"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="target_temperature_not_at_home_max"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="target_temperature_not_at_home_min"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="temperature_unit"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="id_hot_water_demand_profile"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="hot_water_demand_annual"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="hot_water_demand_unit"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="id_appliance_electricity_demand_profile"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="appliance_electricity_demand_annual"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="appliance_electricity_demand_unit"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="id_vehicle_at_home_profile"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="id_vehicle_distance_profile"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -413,14 +414,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
@@ -439,7 +440,7 @@
     <col min="15" max="15" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +487,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -512,7 +513,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>2500000</v>
+        <v>2700</v>
       </c>
       <c r="J2" t="s">
         <v>10</v>
@@ -521,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>4000000</v>
+        <v>1000</v>
       </c>
       <c r="M2" t="s">
         <v>10</v>

</xml_diff>